<commit_message>
se remueven las variables de entorno y se añade archivo .gitignore
</commit_message>
<xml_diff>
--- a/excel_carga_masiva.xlsx
+++ b/excel_carga_masiva.xlsx
@@ -442,10 +442,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>SAMSUNG PM P4049798I</v>
+        <v>SAMSUNG PM P4980809I</v>
       </c>
       <c r="B2" t="str">
-        <v>P4049798I</v>
+        <v>P4980809I</v>
       </c>
       <c r="C2" t="str">
         <v>familycodex</v>
@@ -480,10 +480,10 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>SAMSUNG PM P4049798N</v>
+        <v>SAMSUNG PM P4980809N</v>
       </c>
       <c r="B3" t="str">
-        <v>P4049798N</v>
+        <v>P4980809N</v>
       </c>
       <c r="C3" t="str">
         <v>familycodex</v>
@@ -513,158 +513,6 @@
         <v>true</v>
       </c>
       <c r="L3" t="str">
-        <v>2024-10-07</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>SAMSUNG PM P4049799I</v>
-      </c>
-      <c r="B4" t="str">
-        <v>P4049799I</v>
-      </c>
-      <c r="C4" t="str">
-        <v>familycodex</v>
-      </c>
-      <c r="D4" t="str">
-        <v>Motorola</v>
-      </c>
-      <c r="E4" t="str">
-        <v>X57</v>
-      </c>
-      <c r="F4" t="str">
-        <v>High</v>
-      </c>
-      <c r="G4" t="str">
-        <v>High End A</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Nano SIM</v>
-      </c>
-      <c r="I4" t="str">
-        <v>12 meses</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Si</v>
-      </c>
-      <c r="K4" t="str">
-        <v>true</v>
-      </c>
-      <c r="L4" t="str">
-        <v>2024-10-07</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>SAMSUNG PM P4049799N</v>
-      </c>
-      <c r="B5" t="str">
-        <v>P4049799N</v>
-      </c>
-      <c r="C5" t="str">
-        <v>familycodex</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Motorola</v>
-      </c>
-      <c r="E5" t="str">
-        <v>X58</v>
-      </c>
-      <c r="F5" t="str">
-        <v>High</v>
-      </c>
-      <c r="G5" t="str">
-        <v>High End A</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Nano SIM</v>
-      </c>
-      <c r="I5" t="str">
-        <v>12 meses</v>
-      </c>
-      <c r="J5" t="str">
-        <v>Si</v>
-      </c>
-      <c r="K5" t="str">
-        <v>true</v>
-      </c>
-      <c r="L5" t="str">
-        <v>2024-10-07</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>SAMSUNG PM P4049800N</v>
-      </c>
-      <c r="B6" t="str">
-        <v>P4049800N</v>
-      </c>
-      <c r="C6" t="str">
-        <v>familycodex</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Motorola</v>
-      </c>
-      <c r="E6" t="str">
-        <v>X59</v>
-      </c>
-      <c r="F6" t="str">
-        <v>High</v>
-      </c>
-      <c r="G6" t="str">
-        <v>High End A</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Nano SIM</v>
-      </c>
-      <c r="I6" t="str">
-        <v>12 meses</v>
-      </c>
-      <c r="J6" t="str">
-        <v>Si</v>
-      </c>
-      <c r="K6" t="str">
-        <v>true</v>
-      </c>
-      <c r="L6" t="str">
-        <v>2024-10-07</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>SAMSUNG PM P4049800I</v>
-      </c>
-      <c r="B7" t="str">
-        <v>P4049800I</v>
-      </c>
-      <c r="C7" t="str">
-        <v>familycodex</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Motorola</v>
-      </c>
-      <c r="E7" t="str">
-        <v>X60</v>
-      </c>
-      <c r="F7" t="str">
-        <v>High</v>
-      </c>
-      <c r="G7" t="str">
-        <v>High End A</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Nano SIM</v>
-      </c>
-      <c r="I7" t="str">
-        <v>12 meses</v>
-      </c>
-      <c r="J7" t="str">
-        <v>Si</v>
-      </c>
-      <c r="K7" t="str">
-        <v>true</v>
-      </c>
-      <c r="L7" t="str">
         <v>2024-10-07</v>
       </c>
     </row>

</xml_diff>